<commit_message>
chore(deals): update South of Mound pro forma and summary PDF
</commit_message>
<xml_diff>
--- a/pa-partners-new/public/deals/south-of-mound-pro-forma.xlsx
+++ b/pa-partners-new/public/deals/south-of-mound-pro-forma.xlsx
@@ -432,7 +432,7 @@
         <v>Date:</v>
       </c>
       <c r="B3" t="str">
-        <v>9/25/2025</v>
+        <v>9/26/2025</v>
       </c>
     </row>
     <row r="5">
@@ -597,7 +597,7 @@
         <v>Other Income (Monthly):</v>
       </c>
       <c r="B8">
-        <v>NaN</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -650,7 +650,7 @@
         <v>Other Expenses:</v>
       </c>
       <c r="B16" s="1">
-        <v>5000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="18">
@@ -980,7 +980,7 @@
         <v>Purchase Price</v>
       </c>
       <c r="B4" s="1">
-        <v>1350000</v>
+        <v>1375000</v>
       </c>
     </row>
     <row r="5">
@@ -996,7 +996,7 @@
         <v>Total Project Cost</v>
       </c>
       <c r="B6" s="1">
-        <v>1648000</v>
+        <v>1675500</v>
       </c>
     </row>
     <row r="7">
@@ -1004,7 +1004,7 @@
         <v>Loan Amount</v>
       </c>
       <c r="B7" s="1">
-        <v>1233750</v>
+        <v>1172850</v>
       </c>
     </row>
     <row r="8">
@@ -1036,7 +1036,7 @@
         <v>LTV</v>
       </c>
       <c r="B11" s="2">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="12">
@@ -1060,7 +1060,7 @@
         <v>Preferred Return</v>
       </c>
       <c r="B14" s="2">
-        <v>0.08</v>
+        <v>0.0625</v>
       </c>
     </row>
     <row r="15">
@@ -1076,7 +1076,7 @@
         <v>Year 1 NOI</v>
       </c>
       <c r="B16" s="1">
-        <v>122000</v>
+        <v>124109</v>
       </c>
     </row>
     <row r="17">

</xml_diff>